<commit_message>
Undertstaning of instance variables
Executed Java program in dubg mode and understood the debugging
</commit_message>
<xml_diff>
--- a/arsautomation/src/test/resources/java-flow/ars_data_flow.xlsx
+++ b/arsautomation/src/test/resources/java-flow/ars_data_flow.xlsx
@@ -1,21 +1,99 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HEAP" sheetId="1" r:id="rId1"/>
+    <sheet name="RegistrationOffice" sheetId="2" r:id="rId2"/>
+    <sheet name="LegalEntity" sheetId="3" r:id="rId3"/>
+    <sheet name="Register" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">main()
+</t>
+  </si>
+  <si>
+    <t>LegalEntity le1 = null;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le1 = new LegalEntity("K34612") ; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">public LegalEntity(String tempEntityNumber) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> public void register(double fees)</t>
+  </si>
+  <si>
+    <t>1a1a1001:LegalEntity</t>
+  </si>
+  <si>
+    <t>private int capitalAmount = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> private String name = null;</t>
+  </si>
+  <si>
+    <t>private int shareCount = 0;</t>
+  </si>
+  <si>
+    <t>this=null</t>
+  </si>
+  <si>
+    <t>le1=1a1a1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this.entityNumber=tempEntityNumber; </t>
+  </si>
+  <si>
+    <t>private String entityNumber ="K34612"</t>
+  </si>
+  <si>
+    <t>tempEntityNumber = null</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LegalEntity le2 = null;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> le2 = new LegalEntity("B94000000432") ; </t>
+  </si>
+  <si>
+    <t>1a1a1002:LegalEntity</t>
+  </si>
+  <si>
+    <t>private String entityNumber ="B94000000432"</t>
+  </si>
+  <si>
+    <t>le2=1a1a1002</t>
+  </si>
+  <si>
+    <t>private String entityNumber;</t>
+  </si>
+  <si>
+    <t>private int capitalAmount;</t>
+  </si>
+  <si>
+    <t>private String name ;</t>
+  </si>
+  <si>
+    <t>private int shareCount ;</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,16 +101,64 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,18 +166,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +260,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +295,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,12 +503,244 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="41.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="D18" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
JDBC insert and Select statement
Insert and select statement updated
</commit_message>
<xml_diff>
--- a/arsautomation/src/test/resources/java-flow/ars_data_flow.xlsx
+++ b/arsautomation/src/test/resources/java-flow/ars_data_flow.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HEAP" sheetId="1" r:id="rId1"/>
-    <sheet name="RegistrationOffice" sheetId="2" r:id="rId2"/>
-    <sheet name="LegalEntity" sheetId="3" r:id="rId3"/>
-    <sheet name="Register" sheetId="4" r:id="rId4"/>
+    <sheet name="Stack" sheetId="5" r:id="rId2"/>
+    <sheet name="RegistrationOffice" sheetId="2" r:id="rId3"/>
+    <sheet name="LegalEntity" sheetId="3" r:id="rId4"/>
+    <sheet name="Register" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t xml:space="preserve">main()
 </t>
@@ -38,15 +39,6 @@
     <t>1a1a1001:LegalEntity</t>
   </si>
   <si>
-    <t>private int capitalAmount = 0;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> private String name = null;</t>
-  </si>
-  <si>
-    <t>private int shareCount = 0;</t>
-  </si>
-  <si>
     <t>this=null</t>
   </si>
   <si>
@@ -56,9 +48,6 @@
     <t xml:space="preserve">this.entityNumber=tempEntityNumber; </t>
   </si>
   <si>
-    <t>private String entityNumber ="K34612"</t>
-  </si>
-  <si>
     <t>tempEntityNumber = null</t>
   </si>
   <si>
@@ -71,9 +60,6 @@
     <t>1a1a1002:LegalEntity</t>
   </si>
   <si>
-    <t>private String entityNumber ="B94000000432"</t>
-  </si>
-  <si>
     <t>le2=1a1a1002</t>
   </si>
   <si>
@@ -87,6 +73,141 @@
   </si>
   <si>
     <t>private int shareCount ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">private int capitalAmount </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> private String name </t>
+  </si>
+  <si>
+    <t>private int shareCount</t>
+  </si>
+  <si>
+    <t>private String entityNumber</t>
+  </si>
+  <si>
+    <t>le1</t>
+  </si>
+  <si>
+    <t>Classname</t>
+  </si>
+  <si>
+    <t>Methodname</t>
+  </si>
+  <si>
+    <t>ref.name</t>
+  </si>
+  <si>
+    <t>RegistrationOffice</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>Ref type</t>
+  </si>
+  <si>
+    <t>LegalEntity</t>
+  </si>
+  <si>
+    <t>1a1a1003:LegalEntity</t>
+  </si>
+  <si>
+    <t>1a1a1004:LegalEntity</t>
+  </si>
+  <si>
+    <t>1a1a1005:LegalEntity</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>1b1b7001</t>
+  </si>
+  <si>
+    <t>1b1b7001: LegalEntity[5]</t>
+  </si>
+  <si>
+    <t>LegalEntity[0]</t>
+  </si>
+  <si>
+    <t>LegalEntity[1]</t>
+  </si>
+  <si>
+    <t>1a1a1002</t>
+  </si>
+  <si>
+    <t>LegalEntity[2]</t>
+  </si>
+  <si>
+    <t>LegalEntity[3]</t>
+  </si>
+  <si>
+    <t>1a1a1003</t>
+  </si>
+  <si>
+    <t>1a1a1004</t>
+  </si>
+  <si>
+    <t>1a1a1005</t>
+  </si>
+  <si>
+    <t>LegalEntity[4]</t>
+  </si>
+  <si>
+    <t>6d06d69c:LegalEntity</t>
+  </si>
+  <si>
+    <t>"EN11026"</t>
+  </si>
+  <si>
+    <t>"N-1026"</t>
+  </si>
+  <si>
+    <t>6d06d69c</t>
+  </si>
+  <si>
+    <t>7852e922:LegalEntity</t>
+  </si>
+  <si>
+    <t>"EN11027"</t>
+  </si>
+  <si>
+    <t>"N-1027"</t>
+  </si>
+  <si>
+    <t>le2</t>
+  </si>
+  <si>
+    <t>7852e922</t>
+  </si>
+  <si>
+    <t>1c1c8001</t>
+  </si>
+  <si>
+    <t>1c1c8001:LegalEnitityArrayRepository</t>
+  </si>
+  <si>
+    <t>legalEntities: LegalEntity[]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILegalEntityRepository </t>
+  </si>
+  <si>
+    <t>lerepo</t>
+  </si>
+  <si>
+    <t>Memory location)</t>
+  </si>
+  <si>
+    <t>LegalEnitityArrayRepository</t>
+  </si>
+  <si>
+    <t>insert</t>
+  </si>
+  <si>
+    <t>le</t>
   </si>
 </sst>
 </file>
@@ -108,7 +229,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,8 +278,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -181,11 +314,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -200,6 +346,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,76 +658,384 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B16"/>
+  <dimension ref="B1:J59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.5703125" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" customWidth="1"/>
+    <col min="9" max="9" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+    <row r="1" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="I2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="14">
+        <v>11026</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="14">
+        <v>11027</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="C17" s="6"/>
+      <c r="F17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="F22" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -581,6 +1043,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B10"/>
   <sheetViews>
@@ -610,7 +1178,7 @@
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
@@ -618,17 +1186,17 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -637,11 +1205,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -654,27 +1222,27 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -687,13 +1255,13 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D10" s="5"/>
     </row>
@@ -734,7 +1302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
PageObject related Class are created
</commit_message>
<xml_diff>
--- a/arsautomation/src/test/resources/java-flow/ars_data_flow.xlsx
+++ b/arsautomation/src/test/resources/java-flow/ars_data_flow.xlsx
@@ -9,16 +9,17 @@
   <sheets>
     <sheet name="HEAP" sheetId="1" r:id="rId1"/>
     <sheet name="Stack" sheetId="5" r:id="rId2"/>
-    <sheet name="RegistrationOffice" sheetId="2" r:id="rId3"/>
-    <sheet name="LegalEntity" sheetId="3" r:id="rId4"/>
-    <sheet name="Register" sheetId="4" r:id="rId5"/>
+    <sheet name="LoginPageObject" sheetId="6" r:id="rId3"/>
+    <sheet name="RegistrationOffice" sheetId="2" r:id="rId4"/>
+    <sheet name="LegalEntity" sheetId="3" r:id="rId5"/>
+    <sheet name="Register" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
   <si>
     <t xml:space="preserve">main()
 </t>
@@ -208,6 +209,63 @@
   </si>
   <si>
     <t>le</t>
+  </si>
+  <si>
+    <t>1a1a9001:loginPageObject</t>
+  </si>
+  <si>
+    <t>userID</t>
+  </si>
+  <si>
+    <t>AddLegalEntityUT</t>
+  </si>
+  <si>
+    <t>verifyLEAdditon</t>
+  </si>
+  <si>
+    <t>loginpo</t>
+  </si>
+  <si>
+    <t>LoginPageObject</t>
+  </si>
+  <si>
+    <t>1a1a9001</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>login()</t>
+  </si>
+  <si>
+    <t>1a1a11001</t>
+  </si>
+  <si>
+    <t>1a1a11001: String</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>1a1a11002: String</t>
+  </si>
+  <si>
+    <t>password(admin)</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>1a1a11002</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>1a1a11002:</t>
   </si>
 </sst>
 </file>
@@ -229,7 +287,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +348,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -331,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -354,6 +424,10 @@
     <xf numFmtId="11" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J59"/>
+  <dimension ref="B1:R59"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,11 +743,16 @@
     <col min="2" max="2" width="47.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="35.5703125" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" customWidth="1"/>
     <col min="9" max="9" width="41.85546875" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
         <v>45</v>
       </c>
@@ -682,8 +761,17 @@
         <v>55</v>
       </c>
       <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L2" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="18"/>
+      <c r="P2" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+    </row>
+    <row r="3" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>21</v>
       </c>
@@ -696,43 +784,78 @@
       <c r="J3" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="P3" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" s="21"/>
+    </row>
+    <row r="4" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="14">
         <v>11026</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+    </row>
+    <row r="5" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="P5" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+    </row>
+    <row r="6" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="14">
         <v>1026</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="P6" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="R6" s="21"/>
+    </row>
+    <row r="7" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
-    </row>
-    <row r="8" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+    </row>
+    <row r="8" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+    </row>
+    <row r="9" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="14"/>
     </row>
-    <row r="10" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>21</v>
       </c>
@@ -740,7 +863,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>18</v>
       </c>
@@ -748,7 +871,7 @@
         <v>11027</v>
       </c>
     </row>
-    <row r="12" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
@@ -756,7 +879,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>20</v>
       </c>
@@ -764,15 +887,15 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="14" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
     </row>
-    <row r="15" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
     </row>
-    <row r="16" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>5</v>
@@ -1044,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F5"/>
+  <dimension ref="B1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,12 +1266,137 @@
         <v>33</v>
       </c>
     </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B10"/>
   <sheetViews>
@@ -1205,7 +1453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D18"/>
   <sheetViews>
@@ -1302,7 +1550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>